<commit_message>
Update ompatibilty matrix for Ampoule OSRAM RGB Class 60
</commit_message>
<xml_diff>
--- a/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
+++ b/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="223">
   <si>
     <t>Inclusion</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>Sensor</t>
+  </si>
+  <si>
+    <t>not implemented in NE</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -768,6 +771,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -870,7 +879,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -927,6 +936,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1268,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AY52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1293,7 +1308,7 @@
     <col min="23" max="24" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="37" width="10.5" customWidth="1"/>
-    <col min="38" max="38" width="19.1640625" customWidth="1"/>
+    <col min="38" max="38" width="2.33203125" customWidth="1"/>
     <col min="39" max="39" width="3.33203125" customWidth="1"/>
     <col min="40" max="42" width="17.83203125" customWidth="1"/>
     <col min="43" max="43" width="3.83203125" customWidth="1"/>
@@ -1642,23 +1657,40 @@
       <c r="Z6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AA6" s="10"/>
+      <c r="AA6" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AB6" s="15" t="s">
         <v>60</v>
       </c>
       <c r="AC6" s="15" t="s">
         <v>60</v>
       </c>
+      <c r="AD6" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AE6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
+      <c r="AF6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL6" s="10"/>
       <c r="AM6" s="10"/>
       <c r="AN6" s="15" t="s">
         <v>60</v>
@@ -2155,7 +2187,9 @@
       <c r="L17" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="N17" s="15" t="s">
         <v>58</v>
       </c>
@@ -3260,7 +3294,7 @@
     <row r="52" spans="2:50" ht="15" customHeight="1">
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
-      <c r="D52" s="10"/>
+      <c r="D52" s="24"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>

</xml_diff>

<commit_message>
More info on cap matrix
</commit_message>
<xml_diff>
--- a/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
+++ b/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="980" windowWidth="64880" windowHeight="27260" tabRatio="500"/>
+    <workbookView xWindow="6960" yWindow="8660" windowWidth="64880" windowHeight="27260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$5:$AX$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$5:$AZ$51</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="228">
   <si>
     <t>Inclusion</t>
   </si>
@@ -691,6 +691,21 @@
   </si>
   <si>
     <t>not implemented in NE</t>
+  </si>
+  <si>
+    <t>TRADFRI bulb E14 WS opal 400lm</t>
+  </si>
+  <si>
+    <t>Chaleur</t>
+  </si>
+  <si>
+    <t>30E</t>
+  </si>
+  <si>
+    <t>Identify</t>
+  </si>
+  <si>
+    <t>On+(Off/On)x6</t>
   </si>
 </sst>
 </file>
@@ -1281,10 +1296,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AY52"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="B2:BA52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1293,7 +1309,7 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
@@ -1304,22 +1320,22 @@
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="37" width="10.5" customWidth="1"/>
-    <col min="38" max="38" width="2.33203125" customWidth="1"/>
-    <col min="39" max="39" width="3.33203125" customWidth="1"/>
-    <col min="40" max="42" width="17.83203125" customWidth="1"/>
-    <col min="43" max="43" width="3.83203125" customWidth="1"/>
-    <col min="44" max="47" width="17.1640625" customWidth="1"/>
-    <col min="48" max="48" width="3.83203125" customWidth="1"/>
-    <col min="49" max="49" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.83203125" customWidth="1"/>
+    <col min="24" max="24" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="39" width="10.5" customWidth="1"/>
+    <col min="40" max="40" width="2.33203125" customWidth="1"/>
+    <col min="41" max="41" width="3.33203125" customWidth="1"/>
+    <col min="42" max="44" width="17.83203125" customWidth="1"/>
+    <col min="45" max="45" width="3.83203125" customWidth="1"/>
+    <col min="46" max="49" width="17.1640625" customWidth="1"/>
+    <col min="50" max="50" width="3.83203125" customWidth="1"/>
+    <col min="51" max="51" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:50" ht="15" customHeight="1" thickBot="1"/>
-    <row r="3" spans="2:50" ht="15" customHeight="1">
+    <row r="2" spans="2:52" ht="15" customHeight="1" thickBot="1"/>
+    <row r="3" spans="2:52" ht="15" customHeight="1">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1347,50 +1363,52 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2" t="s">
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2" t="s">
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2" t="s">
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2" t="s">
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2" t="s">
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
-      <c r="AN3" s="2" t="s">
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
       <c r="AQ3" s="2"/>
-      <c r="AR3" s="2" t="s">
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
       <c r="AU3" s="2"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
-      <c r="AX3" s="3"/>
-    </row>
-    <row r="4" spans="2:50" ht="15" customHeight="1">
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="3"/>
+    </row>
+    <row r="4" spans="2:52" ht="15" customHeight="1">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1445,9 +1463,11 @@
       <c r="AU4" s="5"/>
       <c r="AV4" s="5"/>
       <c r="AW4" s="5"/>
-      <c r="AX4" s="6"/>
-    </row>
-    <row r="5" spans="2:50" ht="15" customHeight="1" thickBot="1">
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="5"/>
+      <c r="AZ4" s="6"/>
+    </row>
+    <row r="5" spans="2:52" ht="15" customHeight="1" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1501,98 +1521,104 @@
         <v>28</v>
       </c>
       <c r="T5" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="U5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="V5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="W5" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="X5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="Y5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="Z5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="AA5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Z5" s="8" t="s">
+      <c r="AB5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AC5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AB5" s="8" t="s">
+      <c r="AD5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AC5" s="8" t="s">
+      <c r="AE5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AF5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AE5" s="8" t="s">
+      <c r="AG5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AF5" s="8" t="s">
+      <c r="AH5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AG5" s="8" t="s">
+      <c r="AI5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AH5" s="8" t="s">
+      <c r="AJ5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AI5" s="8" t="s">
+      <c r="AK5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AL5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AM5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="8" t="s">
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AN5" s="8" t="s">
+      <c r="AP5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AO5" s="8" t="s">
+      <c r="AQ5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AP5" s="8" t="s">
+      <c r="AR5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AQ5" s="8" t="s">
+      <c r="AS5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AR5" s="8" t="s">
+      <c r="AT5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AS5" s="8" t="s">
+      <c r="AU5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AT5" s="8" t="s">
+      <c r="AV5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AU5" s="8" t="s">
+      <c r="AW5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AV5" s="8" t="s">
+      <c r="AX5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AW5" s="8" t="s">
+      <c r="AY5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AX5" s="9" t="s">
+      <c r="AZ5" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:50" ht="15" customHeight="1">
+    <row r="6" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="B6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1641,25 +1667,21 @@
       <c r="S6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T6" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T6" s="15"/>
       <c r="U6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" s="10"/>
-      <c r="W6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W6" s="15"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X6" s="15" t="s">
+      <c r="Z6" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Z6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA6" s="15" t="s">
-        <v>60</v>
-      </c>
       <c r="AB6" s="15" t="s">
         <v>60</v>
       </c>
@@ -1672,11 +1694,11 @@
       <c r="AE6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AF6" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG6" s="25" t="s">
-        <v>61</v>
+      <c r="AF6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG6" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="AH6" s="25" t="s">
         <v>61</v>
@@ -1690,24 +1712,30 @@
       <c r="AK6" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="AL6" s="10"/>
-      <c r="AM6" s="10"/>
-      <c r="AN6" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AL6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN6" s="10"/>
       <c r="AO6" s="10"/>
-      <c r="AP6" s="10"/>
-      <c r="AR6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AS6" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AP6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
       <c r="AT6" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="2:50" ht="15" customHeight="1">
+      <c r="AU6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV6" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
@@ -1740,37 +1768,39 @@
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
       <c r="U7" s="16"/>
-      <c r="V7" s="17"/>
+      <c r="V7" s="16"/>
       <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="18"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="16"/>
       <c r="Z7" s="16"/>
-      <c r="AA7" s="17"/>
+      <c r="AA7" s="18"/>
       <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="18"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="16"/>
       <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
+      <c r="AF7" s="18"/>
       <c r="AG7" s="16"/>
       <c r="AH7" s="16"/>
       <c r="AI7" s="16"/>
       <c r="AJ7" s="16"/>
       <c r="AK7" s="16"/>
       <c r="AL7" s="16"/>
-      <c r="AM7" s="17"/>
+      <c r="AM7" s="16"/>
       <c r="AN7" s="16"/>
       <c r="AO7" s="17"/>
-      <c r="AP7" s="17"/>
-      <c r="AQ7" s="18"/>
-      <c r="AR7" s="16"/>
-      <c r="AS7" s="16"/>
+      <c r="AP7" s="16"/>
+      <c r="AQ7" s="17"/>
+      <c r="AR7" s="17"/>
+      <c r="AS7" s="18"/>
       <c r="AT7" s="16"/>
-      <c r="AU7" s="18"/>
-      <c r="AV7" s="18"/>
+      <c r="AU7" s="16"/>
+      <c r="AV7" s="16"/>
       <c r="AW7" s="18"/>
       <c r="AX7" s="18"/>
-    </row>
-    <row r="8" spans="2:50" ht="15" customHeight="1">
+      <c r="AY7" s="18"/>
+      <c r="AZ7" s="18"/>
+    </row>
+    <row r="8" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="10" t="s">
@@ -1803,37 +1833,39 @@
       <c r="S8" s="16"/>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
-      <c r="V8" s="17"/>
+      <c r="V8" s="16"/>
       <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="18"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="16"/>
       <c r="Z8" s="16"/>
-      <c r="AA8" s="17"/>
+      <c r="AA8" s="18"/>
       <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="18"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="16"/>
       <c r="AE8" s="16"/>
-      <c r="AF8" s="16"/>
+      <c r="AF8" s="18"/>
       <c r="AG8" s="16"/>
       <c r="AH8" s="16"/>
       <c r="AI8" s="16"/>
       <c r="AJ8" s="16"/>
       <c r="AK8" s="16"/>
       <c r="AL8" s="16"/>
-      <c r="AM8" s="17"/>
+      <c r="AM8" s="16"/>
       <c r="AN8" s="16"/>
       <c r="AO8" s="17"/>
-      <c r="AP8" s="17"/>
-      <c r="AQ8" s="18"/>
-      <c r="AR8" s="16"/>
-      <c r="AS8" s="16"/>
+      <c r="AP8" s="16"/>
+      <c r="AQ8" s="17"/>
+      <c r="AR8" s="17"/>
+      <c r="AS8" s="18"/>
       <c r="AT8" s="16"/>
-      <c r="AU8" s="18"/>
-      <c r="AV8" s="18"/>
+      <c r="AU8" s="16"/>
+      <c r="AV8" s="16"/>
       <c r="AW8" s="18"/>
       <c r="AX8" s="18"/>
-    </row>
-    <row r="9" spans="2:50" ht="15" customHeight="1">
+      <c r="AY8" s="18"/>
+      <c r="AZ8" s="18"/>
+    </row>
+    <row r="9" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D9" s="10" t="s">
         <v>71</v>
       </c>
@@ -1853,7 +1885,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:50" ht="15" customHeight="1">
+    <row r="10" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D10" s="10" t="s">
         <v>75</v>
       </c>
@@ -1873,7 +1905,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:50" ht="15" customHeight="1">
+    <row r="11" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D11" s="10" t="s">
         <v>75</v>
       </c>
@@ -1893,7 +1925,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="2:50" ht="15" customHeight="1">
+    <row r="12" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D12" s="10" t="s">
         <v>80</v>
       </c>
@@ -1913,7 +1945,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="2:50" ht="15" customHeight="1">
+    <row r="13" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="B13" s="10" t="s">
         <v>84</v>
       </c>
@@ -1958,54 +1990,56 @@
       <c r="S13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T13" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T13" s="15"/>
       <c r="U13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V13" s="10"/>
-      <c r="W13" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="V13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W13" s="15"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X13" s="15" t="s">
+      <c r="Z13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="19" t="s">
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="AA13" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB13" s="20" t="s">
-        <v>92</v>
       </c>
       <c r="AC13" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AD13" s="19" t="s">
+      <c r="AD13" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE13" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AE13" s="20" t="s">
+      <c r="AF13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG13" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AF13" s="20"/>
-      <c r="AG13" s="20"/>
       <c r="AH13" s="20"/>
       <c r="AI13" s="20"/>
       <c r="AJ13" s="20"/>
       <c r="AK13" s="20"/>
       <c r="AL13" s="20"/>
-      <c r="AM13" s="10"/>
-      <c r="AN13" s="10"/>
+      <c r="AM13" s="20"/>
+      <c r="AN13" s="20"/>
       <c r="AO13" s="10"/>
       <c r="AP13" s="10"/>
-      <c r="AW13" s="21" t="s">
+      <c r="AQ13" s="10"/>
+      <c r="AR13" s="10"/>
+      <c r="AY13" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:50" ht="15" customHeight="1">
+    <row r="14" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D14" s="10" t="s">
         <v>85</v>
       </c>
@@ -2025,7 +2059,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="2:50" ht="15" customHeight="1">
+    <row r="15" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="B15" s="10" t="s">
         <v>84</v>
       </c>
@@ -2070,51 +2104,53 @@
       <c r="S15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T15" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T15" s="15"/>
       <c r="U15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V15" s="10"/>
-      <c r="W15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W15" s="15"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X15" s="15" t="s">
+      <c r="Z15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="19" t="s">
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="AA15" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB15" s="20" t="s">
-        <v>92</v>
       </c>
       <c r="AC15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AD15" s="19" t="s">
+      <c r="AD15" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AE15" s="20" t="s">
+      <c r="AF15" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG15" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AF15" s="20"/>
-      <c r="AG15" s="20"/>
       <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
       <c r="AJ15" s="20"/>
       <c r="AK15" s="20"/>
       <c r="AL15" s="20"/>
-      <c r="AM15" s="10"/>
-      <c r="AN15" s="10"/>
+      <c r="AM15" s="20"/>
+      <c r="AN15" s="20"/>
       <c r="AO15" s="10"/>
       <c r="AP15" s="10"/>
-    </row>
-    <row r="16" spans="2:50" ht="15" customHeight="1">
+      <c r="AQ15" s="10"/>
+      <c r="AR15" s="10"/>
+    </row>
+    <row r="16" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D16" s="10" t="s">
         <v>75</v>
       </c>
@@ -2140,26 +2176,28 @@
       <c r="S16" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="16" t="s">
-        <v>61</v>
-      </c>
+      <c r="T16" s="15"/>
       <c r="U16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="AB16" s="22" t="s">
+      <c r="V16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="W16" s="16"/>
+      <c r="AD16" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="AE16" s="22" t="s">
+      <c r="AG16" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="AH16" s="22" t="s">
+      <c r="AJ16" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="AK16" s="22" t="s">
+      <c r="AM16" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="2:51" ht="15" customHeight="1">
+    <row r="17" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="B17" s="10" t="s">
         <v>50</v>
       </c>
@@ -2206,24 +2244,20 @@
       <c r="S17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T17" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="T17" s="15"/>
       <c r="U17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="V17" s="10"/>
-      <c r="W17" s="15" t="s">
+      <c r="V17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W17" s="15"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X17" s="15" t="s">
-        <v>61</v>
-      </c>
       <c r="Z17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA17" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB17" s="15" t="s">
         <v>60</v>
@@ -2237,37 +2271,43 @@
       <c r="AE17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AF17" s="15"/>
-      <c r="AG17" s="15"/>
+      <c r="AF17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG17" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AH17" s="15"/>
       <c r="AI17" s="15"/>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>
       <c r="AL17" s="15"/>
-      <c r="AM17" s="10"/>
-      <c r="AN17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO17" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="10"/>
       <c r="AP17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AQ17" s="10"/>
-      <c r="AR17" s="10"/>
+      <c r="AQ17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR17" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AS17" s="10"/>
       <c r="AT17" s="10"/>
+      <c r="AU17" s="10"/>
       <c r="AV17" s="10"/>
-      <c r="AW17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AY17" s="10"/>
-    </row>
-    <row r="18" spans="2:51" ht="15" customHeight="1">
+      <c r="AX17" s="10"/>
+      <c r="AY17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BA17" s="10"/>
+    </row>
+    <row r="18" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D18" s="10" t="s">
         <v>85</v>
       </c>
@@ -2285,7 +2325,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:51" ht="15" customHeight="1">
+    <row r="19" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D19" s="10" t="s">
         <v>75</v>
       </c>
@@ -2305,7 +2345,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="2:51" ht="15" customHeight="1">
+    <row r="20" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D20" s="12" t="s">
         <v>75</v>
       </c>
@@ -2325,7 +2365,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="2:51" ht="15" customHeight="1">
+    <row r="21" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D21" s="12" t="s">
         <v>75</v>
       </c>
@@ -2345,7 +2385,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="2:51" ht="15" customHeight="1">
+    <row r="22" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D22" s="10" t="s">
         <v>75</v>
       </c>
@@ -2365,7 +2405,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="2:51" ht="15" customHeight="1">
+    <row r="23" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D23" s="10" t="s">
         <v>75</v>
       </c>
@@ -2385,7 +2425,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="2:51" ht="15" customHeight="1">
+    <row r="24" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D24" s="10" t="s">
         <v>75</v>
       </c>
@@ -2405,7 +2445,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="2:51" ht="15" customHeight="1">
+    <row r="25" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D25" s="10" t="s">
         <v>75</v>
       </c>
@@ -2425,7 +2465,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="2:51" ht="15" customHeight="1">
+    <row r="26" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D26" s="10" t="s">
         <v>75</v>
       </c>
@@ -2445,7 +2485,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="2:51" ht="15" customHeight="1">
+    <row r="27" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D27" s="10" t="s">
         <v>75</v>
       </c>
@@ -2465,7 +2505,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:51" ht="15" customHeight="1">
+    <row r="28" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D28" s="10" t="s">
         <v>75</v>
       </c>
@@ -2485,7 +2525,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:51" ht="15" customHeight="1">
+    <row r="29" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D29" s="10" t="s">
         <v>75</v>
       </c>
@@ -2513,26 +2553,22 @@
       <c r="S29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="T29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="U29" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="V29" s="10"/>
-      <c r="W29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="X29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="V29" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W29" s="15"/>
+      <c r="X29" s="10"/>
+      <c r="Y29" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="Z29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AA29" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AA29" s="10"/>
       <c r="AB29" s="10" t="s">
         <v>61</v>
       </c>
@@ -2545,36 +2581,42 @@
       <c r="AE29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AF29" s="10"/>
-      <c r="AG29" s="10"/>
+      <c r="AF29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG29" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="AH29" s="10"/>
       <c r="AI29" s="10"/>
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
-      <c r="AN29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO29" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AM29" s="10"/>
+      <c r="AN29" s="10"/>
       <c r="AP29" s="10" t="s">
         <v>61</v>
       </c>
+      <c r="AQ29" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="AR29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AS29" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="AT29" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AU29" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="2:51" ht="15" customHeight="1">
+      <c r="AV29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW29" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D30" s="10" t="s">
         <v>75</v>
       </c>
@@ -2615,26 +2657,22 @@
       <c r="S30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="T30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="U30" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="V30" s="10"/>
-      <c r="W30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="X30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="V30" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W30" s="15"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="Z30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AA30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AA30" s="10"/>
       <c r="AB30" s="10" t="s">
         <v>61</v>
       </c>
@@ -2647,37 +2685,43 @@
       <c r="AE30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AF30" s="10"/>
-      <c r="AG30" s="10"/>
+      <c r="AF30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG30" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="AH30" s="10"/>
       <c r="AI30" s="10"/>
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="10"/>
       <c r="AM30" s="10"/>
-      <c r="AN30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AN30" s="10"/>
+      <c r="AO30" s="10"/>
       <c r="AP30" s="10" t="s">
         <v>61</v>
       </c>
+      <c r="AQ30" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="AR30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AS30" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="AT30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AU30" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="2:51" ht="15" customHeight="1">
+      <c r="AV30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW30" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D31" s="10" t="s">
         <v>75</v>
       </c>
@@ -2697,7 +2741,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="2:51" ht="15" customHeight="1">
+    <row r="32" spans="2:53" ht="15" hidden="1" customHeight="1">
       <c r="D32" s="10" t="s">
         <v>75</v>
       </c>
@@ -2717,7 +2761,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="2:42" ht="15" customHeight="1">
+    <row r="33" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D33" s="10" t="s">
         <v>75</v>
       </c>
@@ -2737,7 +2781,10 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="2:42" ht="15" customHeight="1">
+    <row r="34" spans="2:44" ht="15" customHeight="1">
+      <c r="B34" t="s">
+        <v>225</v>
+      </c>
       <c r="D34" s="10" t="s">
         <v>162</v>
       </c>
@@ -2753,11 +2800,86 @@
       <c r="H34" t="s">
         <v>219</v>
       </c>
+      <c r="I34" t="s">
+        <v>227</v>
+      </c>
       <c r="L34" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="35" spans="2:42" ht="15" customHeight="1">
+        <v>223</v>
+      </c>
+      <c r="M34" t="s">
+        <v>222</v>
+      </c>
+      <c r="N34" t="s">
+        <v>60</v>
+      </c>
+      <c r="O34" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>60</v>
+      </c>
+      <c r="R34" t="s">
+        <v>60</v>
+      </c>
+      <c r="S34" t="s">
+        <v>60</v>
+      </c>
+      <c r="T34" t="s">
+        <v>60</v>
+      </c>
+      <c r="U34" t="s">
+        <v>61</v>
+      </c>
+      <c r="V34" t="s">
+        <v>61</v>
+      </c>
+      <c r="W34" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="B35" s="10" t="s">
         <v>84</v>
       </c>
@@ -2802,51 +2924,53 @@
       <c r="S35" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T35" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T35" s="15"/>
       <c r="U35" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V35" s="10"/>
-      <c r="W35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="V35" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W35" s="15"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X35" s="15" t="s">
+      <c r="Z35" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y35" s="10"/>
-      <c r="Z35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA35" s="20" t="s">
+      <c r="AA35" s="10"/>
+      <c r="AB35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC35" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="AB35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD35" s="20" t="s">
+      <c r="AD35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF35" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="AE35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF35" s="15"/>
-      <c r="AG35" s="15"/>
+      <c r="AG35" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AH35" s="15"/>
       <c r="AI35" s="15"/>
       <c r="AJ35" s="15"/>
       <c r="AK35" s="15"/>
       <c r="AL35" s="15"/>
-      <c r="AM35" s="10"/>
-      <c r="AN35" s="10"/>
+      <c r="AM35" s="15"/>
+      <c r="AN35" s="15"/>
       <c r="AO35" s="10"/>
       <c r="AP35" s="10"/>
-    </row>
-    <row r="36" spans="2:42" ht="15" customHeight="1">
+      <c r="AQ35" s="10"/>
+      <c r="AR35" s="10"/>
+    </row>
+    <row r="36" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D36" s="10" t="s">
         <v>162</v>
       </c>
@@ -2866,7 +2990,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="2:42" ht="15" customHeight="1">
+    <row r="37" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D37" s="10" t="s">
         <v>162</v>
       </c>
@@ -2886,7 +3010,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="2:42" ht="15" customHeight="1">
+    <row r="38" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D38" s="10" t="s">
         <v>162</v>
       </c>
@@ -2906,7 +3030,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="2:42" ht="15" customHeight="1">
+    <row r="39" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D39" s="10" t="s">
         <v>162</v>
       </c>
@@ -2926,7 +3050,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="2:42" ht="15" customHeight="1">
+    <row r="40" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D40" s="10" t="s">
         <v>162</v>
       </c>
@@ -2946,7 +3070,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="2:42" ht="15" customHeight="1">
+    <row r="41" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D41" s="10" t="s">
         <v>162</v>
       </c>
@@ -2966,7 +3090,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="2:42" ht="15" customHeight="1">
+    <row r="42" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D42" s="10" t="s">
         <v>162</v>
       </c>
@@ -2986,7 +3110,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="43" spans="2:42" ht="15" customHeight="1">
+    <row r="43" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D43" s="10" t="s">
         <v>162</v>
       </c>
@@ -3006,7 +3130,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="2:42" ht="15" customHeight="1">
+    <row r="44" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D44" s="10" t="s">
         <v>162</v>
       </c>
@@ -3026,7 +3150,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="2:42" ht="15" customHeight="1">
+    <row r="45" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D45" s="10" t="s">
         <v>75</v>
       </c>
@@ -3046,7 +3170,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="2:42" ht="15" customHeight="1">
+    <row r="46" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="B46" s="10"/>
       <c r="C46" s="11">
         <v>43273</v>
@@ -3087,33 +3211,35 @@
       <c r="S46" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T46" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="T46" s="15"/>
       <c r="U46" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="V46" s="10"/>
-      <c r="W46" s="15" t="s">
+      <c r="V46" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W46" s="15"/>
+      <c r="X46" s="10"/>
+      <c r="Y46" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X46" s="15" t="s">
+      <c r="Z46" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="Y46" s="10"/>
-      <c r="Z46" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="AA46" s="10"/>
       <c r="AB46" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AM46" s="10"/>
-      <c r="AN46" s="10"/>
+      <c r="AC46" s="10"/>
+      <c r="AD46" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AO46" s="10"/>
       <c r="AP46" s="10"/>
-    </row>
-    <row r="47" spans="2:42" ht="15" customHeight="1">
+      <c r="AQ46" s="10"/>
+      <c r="AR46" s="10"/>
+    </row>
+    <row r="47" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="D47" s="10" t="s">
         <v>75</v>
       </c>
@@ -3133,7 +3259,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="2:42" ht="15" customHeight="1">
+    <row r="48" spans="2:44" ht="15" hidden="1" customHeight="1">
       <c r="B48" s="10" t="s">
         <v>84</v>
       </c>
@@ -3175,52 +3301,54 @@
       <c r="S48" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T48" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="T48" s="15"/>
       <c r="U48" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="V48" s="10"/>
-      <c r="W48" s="15" t="s">
+      <c r="V48" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W48" s="15"/>
+      <c r="X48" s="10"/>
+      <c r="Y48" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X48" s="15" t="s">
+      <c r="Z48" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="Y48" s="10"/>
-      <c r="Z48" s="10"/>
-      <c r="AA48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC48" s="23" t="s">
-        <v>214</v>
+      <c r="AA48" s="10"/>
+      <c r="AB48" s="10"/>
+      <c r="AC48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD48" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="AE48" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="AF48" s="15"/>
-      <c r="AG48" s="15"/>
+      <c r="AG48" s="23" t="s">
+        <v>214</v>
+      </c>
       <c r="AH48" s="15"/>
       <c r="AI48" s="15"/>
       <c r="AJ48" s="15"/>
       <c r="AK48" s="15"/>
       <c r="AL48" s="15"/>
-      <c r="AM48" s="10"/>
-      <c r="AN48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO48" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AM48" s="15"/>
+      <c r="AN48" s="15"/>
+      <c r="AO48" s="10"/>
       <c r="AP48" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="2:50" ht="15" customHeight="1">
+      <c r="AQ48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AR48" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D49" s="10" t="s">
         <v>208</v>
       </c>
@@ -3240,7 +3368,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="50" spans="2:50" ht="15" customHeight="1">
+    <row r="50" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="D50" s="10" t="s">
         <v>208</v>
       </c>
@@ -3262,14 +3390,14 @@
       <c r="L50" t="s">
         <v>216</v>
       </c>
-      <c r="AW50" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX50" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="2:50" ht="15" customHeight="1">
+      <c r="AY50" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ50" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:52" ht="15" hidden="1" customHeight="1">
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="10" t="s">
@@ -3291,7 +3419,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="52" spans="2:50" ht="15" customHeight="1">
+    <row r="52" spans="2:52" ht="15" customHeight="1">
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
       <c r="D52" s="24"/>
@@ -3309,7 +3437,18 @@
       <c r="P52" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:AX50"/>
+  <autoFilter ref="B5:AZ51">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Ikea"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter val="*E14*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Bit more compat matrix info
</commit_message>
<xml_diff>
--- a/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
+++ b/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$5:$AZ$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$5:$BA$51</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="233">
   <si>
     <t>Inclusion</t>
   </si>
@@ -366,9 +366,6 @@
     <t>lumi.sensor_86sw2</t>
   </si>
   <si>
-    <t>sensor_86sw3</t>
-  </si>
-  <si>
     <t>Xiaomi Interrupteur Mural Carré Double</t>
   </si>
   <si>
@@ -709,6 +706,21 @@
   </si>
   <si>
     <t>Yes (On/Off/Level)</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>ZNCZ02LM</t>
+  </si>
+  <si>
+    <t>wxkg02LM</t>
+  </si>
+  <si>
+    <t>lumi.sensor_86sw2Un</t>
+  </si>
+  <si>
+    <t>sensor_86sw2Un</t>
   </si>
 </sst>
 </file>
@@ -888,12 +900,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -965,14 +981,18 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="40 % - Accent1" xfId="4" builtinId="31" customBuiltin="1"/>
     <cellStyle name="Bon" xfId="1" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Neutre" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -1303,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:BA52"/>
+  <dimension ref="B2:BB52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1315,33 +1335,34 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.83203125" customWidth="1"/>
-    <col min="12" max="12" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="39" width="10.5" customWidth="1"/>
-    <col min="40" max="40" width="2.33203125" customWidth="1"/>
-    <col min="41" max="41" width="3.33203125" customWidth="1"/>
-    <col min="42" max="44" width="17.83203125" customWidth="1"/>
-    <col min="45" max="45" width="3.83203125" customWidth="1"/>
-    <col min="46" max="49" width="17.1640625" customWidth="1"/>
-    <col min="50" max="50" width="3.83203125" customWidth="1"/>
-    <col min="51" max="51" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" customWidth="1"/>
+    <col min="13" max="13" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="40" width="10.5" customWidth="1"/>
+    <col min="41" max="41" width="2.33203125" customWidth="1"/>
+    <col min="42" max="42" width="3.33203125" customWidth="1"/>
+    <col min="43" max="45" width="17.83203125" customWidth="1"/>
+    <col min="46" max="46" width="3.83203125" customWidth="1"/>
+    <col min="47" max="50" width="17.1640625" customWidth="1"/>
+    <col min="51" max="51" width="3.83203125" customWidth="1"/>
+    <col min="52" max="52" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:52" ht="15" customHeight="1" thickBot="1"/>
-    <row r="3" spans="2:52" ht="15" customHeight="1">
+    <row r="2" spans="2:53" ht="15" customHeight="1" thickBot="1"/>
+    <row r="3" spans="2:53" ht="15" customHeight="1">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1349,72 +1370,73 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
-      <c r="Y3" s="2" t="s">
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
-      <c r="AB3" s="2" t="s">
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="2" t="s">
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="2" t="s">
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
-      <c r="AK3" s="2" t="s">
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
       <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
-      <c r="AP3" s="2" t="s">
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="2"/>
       <c r="AR3" s="2"/>
       <c r="AS3" s="2"/>
-      <c r="AT3" s="2" t="s">
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AU3" s="2"/>
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
-      <c r="AZ3" s="3"/>
-    </row>
-    <row r="4" spans="2:52" ht="15" customHeight="1">
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="3"/>
+    </row>
+    <row r="4" spans="2:53" ht="15" customHeight="1">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1425,17 +1447,17 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
@@ -1471,9 +1493,10 @@
       <c r="AW4" s="5"/>
       <c r="AX4" s="5"/>
       <c r="AY4" s="5"/>
-      <c r="AZ4" s="6"/>
-    </row>
-    <row r="5" spans="2:52" ht="15" customHeight="1" thickBot="1">
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="6"/>
+    </row>
+    <row r="5" spans="2:53" ht="15" customHeight="1" thickBot="1">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1487,144 +1510,147 @@
         <v>16</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
-        <v>218</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" t="s">
+        <v>217</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="S5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="T5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="8" t="s">
-        <v>224</v>
-      </c>
       <c r="U5" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="V5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="W5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="W5" s="8" t="s">
-        <v>226</v>
-      </c>
       <c r="X5" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Z5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Z5" s="8" t="s">
+      <c r="AA5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AB5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AB5" s="8" t="s">
+      <c r="AC5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AC5" s="8" t="s">
+      <c r="AD5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AE5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AE5" s="8" t="s">
+      <c r="AF5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AF5" s="8" t="s">
+      <c r="AG5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AG5" s="8" t="s">
+      <c r="AH5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AH5" s="8" t="s">
+      <c r="AI5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AI5" s="8" t="s">
+      <c r="AJ5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AJ5" s="8" t="s">
+      <c r="AK5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AL5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="8" t="s">
+      <c r="AM5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AM5" s="8" t="s">
+      <c r="AN5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8" t="s">
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AP5" s="8" t="s">
+      <c r="AQ5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AQ5" s="8" t="s">
+      <c r="AR5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AR5" s="8" t="s">
+      <c r="AS5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AS5" s="8" t="s">
+      <c r="AT5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AT5" s="8" t="s">
+      <c r="AU5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AU5" s="8" t="s">
+      <c r="AV5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AV5" s="8" t="s">
+      <c r="AW5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AW5" s="8" t="s">
+      <c r="AX5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AX5" s="8" t="s">
+      <c r="AY5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AY5" s="8" t="s">
+      <c r="AZ5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AZ5" s="9" t="s">
+      <c r="BA5" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:52" ht="15" customHeight="1">
+    <row r="6" spans="2:53" ht="15" customHeight="1">
       <c r="B6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1637,60 +1663,58 @@
       <c r="E6" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H6" t="s">
-        <v>219</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" t="s">
+        <v>218</v>
+      </c>
+      <c r="J6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="10"/>
+      <c r="M6" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="15"/>
+      <c r="O6" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="P6" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="Q6" s="10"/>
       <c r="R6" s="15" t="s">
         <v>60</v>
       </c>
       <c r="S6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U6" s="15"/>
       <c r="V6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="W6" s="15"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z6" s="15" t="s">
+      <c r="AA6" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AB6" s="15" t="s">
-        <v>60</v>
-      </c>
       <c r="AC6" s="15" t="s">
         <v>60</v>
       </c>
@@ -1706,8 +1730,8 @@
       <c r="AG6" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AH6" s="25" t="s">
-        <v>61</v>
+      <c r="AH6" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="AI6" s="25" t="s">
         <v>61</v>
@@ -1724,24 +1748,27 @@
       <c r="AM6" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="AN6" s="10"/>
+      <c r="AN6" s="25" t="s">
+        <v>61</v>
+      </c>
       <c r="AO6" s="10"/>
-      <c r="AP6" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AR6" s="10"/>
-      <c r="AT6" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AS6" s="10"/>
       <c r="AU6" s="15" t="s">
         <v>60</v>
       </c>
       <c r="AV6" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="2:52" ht="15" customHeight="1">
+      <c r="AW6" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:53" ht="15" customHeight="1">
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
@@ -1750,42 +1777,42 @@
       <c r="E7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H7" t="s">
-        <v>219</v>
-      </c>
-      <c r="I7" s="10"/>
+      <c r="I7" t="s">
+        <v>218</v>
+      </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="10"/>
+      <c r="M7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="16"/>
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="17"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
       <c r="T7" s="16"/>
       <c r="U7" s="16"/>
       <c r="V7" s="16"/>
       <c r="W7" s="16"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="17"/>
       <c r="Z7" s="16"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="17"/>
-      <c r="AD7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="17"/>
       <c r="AE7" s="16"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="18"/>
       <c r="AH7" s="16"/>
       <c r="AI7" s="16"/>
       <c r="AJ7" s="16"/>
@@ -1793,20 +1820,21 @@
       <c r="AL7" s="16"/>
       <c r="AM7" s="16"/>
       <c r="AN7" s="16"/>
-      <c r="AO7" s="17"/>
-      <c r="AP7" s="16"/>
-      <c r="AQ7" s="17"/>
+      <c r="AO7" s="16"/>
+      <c r="AP7" s="17"/>
+      <c r="AQ7" s="16"/>
       <c r="AR7" s="17"/>
-      <c r="AS7" s="18"/>
-      <c r="AT7" s="16"/>
+      <c r="AS7" s="17"/>
+      <c r="AT7" s="18"/>
       <c r="AU7" s="16"/>
       <c r="AV7" s="16"/>
-      <c r="AW7" s="18"/>
+      <c r="AW7" s="16"/>
       <c r="AX7" s="18"/>
       <c r="AY7" s="18"/>
       <c r="AZ7" s="18"/>
-    </row>
-    <row r="8" spans="2:52" ht="15" customHeight="1">
+      <c r="BA7" s="18"/>
+    </row>
+    <row r="8" spans="2:53" ht="15" customHeight="1">
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="10" t="s">
@@ -1815,42 +1843,42 @@
       <c r="E8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H8" t="s">
-        <v>219</v>
-      </c>
-      <c r="I8" s="10"/>
+      <c r="I8" t="s">
+        <v>218</v>
+      </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="16"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="17"/>
       <c r="R8" s="16"/>
       <c r="S8" s="16"/>
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
       <c r="V8" s="16"/>
       <c r="W8" s="16"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="17"/>
       <c r="Z8" s="16"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="17"/>
-      <c r="AD8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="17"/>
       <c r="AE8" s="16"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="16"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="18"/>
       <c r="AH8" s="16"/>
       <c r="AI8" s="16"/>
       <c r="AJ8" s="16"/>
@@ -1858,100 +1886,105 @@
       <c r="AL8" s="16"/>
       <c r="AM8" s="16"/>
       <c r="AN8" s="16"/>
-      <c r="AO8" s="17"/>
-      <c r="AP8" s="16"/>
-      <c r="AQ8" s="17"/>
+      <c r="AO8" s="16"/>
+      <c r="AP8" s="17"/>
+      <c r="AQ8" s="16"/>
       <c r="AR8" s="17"/>
-      <c r="AS8" s="18"/>
-      <c r="AT8" s="16"/>
+      <c r="AS8" s="17"/>
+      <c r="AT8" s="18"/>
       <c r="AU8" s="16"/>
       <c r="AV8" s="16"/>
-      <c r="AW8" s="18"/>
+      <c r="AW8" s="16"/>
       <c r="AX8" s="18"/>
       <c r="AY8" s="18"/>
       <c r="AZ8" s="18"/>
-    </row>
-    <row r="9" spans="2:52" ht="15" customHeight="1">
+      <c r="BA8" s="18"/>
+    </row>
+    <row r="9" spans="2:53" ht="15" customHeight="1">
       <c r="D9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H9" t="s">
-        <v>220</v>
-      </c>
-      <c r="L9" s="10" t="s">
+      <c r="I9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:52" ht="15" customHeight="1">
+    <row r="10" spans="2:53" ht="15" customHeight="1">
       <c r="D10" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H10" t="s">
-        <v>219</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="I10" t="s">
+        <v>218</v>
+      </c>
+      <c r="M10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:52" ht="15" customHeight="1">
+    <row r="11" spans="2:53" ht="15" customHeight="1">
       <c r="D11" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H11" t="s">
-        <v>219</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="I11" t="s">
+        <v>218</v>
+      </c>
+      <c r="M11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="2:52" ht="15" customHeight="1">
+    <row r="12" spans="2:53" ht="15" customHeight="1">
       <c r="D12" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="H12" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="H12" t="s">
-        <v>220</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="I12" t="s">
+        <v>219</v>
+      </c>
+      <c r="M12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="2:52" ht="15" customHeight="1">
+    <row r="13" spans="2:53" ht="15" customHeight="1">
       <c r="B13" s="10" t="s">
         <v>84</v>
       </c>
@@ -1964,108 +1997,110 @@
       <c r="E13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="H13" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="H13" t="s">
-        <v>219</v>
-      </c>
-      <c r="I13" s="10"/>
+      <c r="I13" t="s">
+        <v>218</v>
+      </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="10"/>
+      <c r="M13" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15" t="s">
+      <c r="N13" s="15"/>
+      <c r="O13" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="P13" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="Q13" s="10"/>
       <c r="R13" s="15" t="s">
         <v>60</v>
       </c>
       <c r="S13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T13" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U13" s="15"/>
       <c r="V13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="W13" s="15"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z13" s="15" t="s">
+      <c r="AA13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="19" t="s">
-        <v>91</v>
-      </c>
+      <c r="AB13" s="10"/>
       <c r="AC13" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AD13" s="20" t="s">
+      <c r="AD13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE13" s="20" t="s">
         <v>92</v>
-      </c>
-      <c r="AE13" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="AF13" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AG13" s="20" t="s">
+      <c r="AG13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH13" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AH13" s="20"/>
       <c r="AI13" s="20"/>
       <c r="AJ13" s="20"/>
       <c r="AK13" s="20"/>
       <c r="AL13" s="20"/>
       <c r="AM13" s="20"/>
       <c r="AN13" s="20"/>
-      <c r="AO13" s="10"/>
+      <c r="AO13" s="20"/>
       <c r="AP13" s="10"/>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="10"/>
-      <c r="AY13" s="21" t="s">
+      <c r="AS13" s="10"/>
+      <c r="AZ13" s="21" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:52" ht="15" customHeight="1">
+    <row r="14" spans="2:53" ht="15" customHeight="1">
       <c r="D14" s="10" t="s">
         <v>85</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="H14" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H14" t="s">
-        <v>219</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="I14" t="s">
+        <v>218</v>
+      </c>
+      <c r="M14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="2:52" ht="15" customHeight="1">
+    <row r="15" spans="2:53" ht="15" customHeight="1">
       <c r="B15" s="10" t="s">
         <v>84</v>
       </c>
@@ -2078,132 +2113,136 @@
       <c r="E15" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="H15" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15" s="10"/>
+      <c r="I15" t="s">
+        <v>218</v>
+      </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="10"/>
+      <c r="M15" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15" t="s">
+      <c r="N15" s="15"/>
+      <c r="O15" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="P15" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="Q15" s="10"/>
       <c r="R15" s="15" t="s">
         <v>60</v>
       </c>
       <c r="S15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="T15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U15" s="15"/>
       <c r="V15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="W15" s="15"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z15" s="15" t="s">
+      <c r="AA15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="19" t="s">
-        <v>91</v>
-      </c>
+      <c r="AB15" s="10"/>
       <c r="AC15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AD15" s="20" t="s">
+      <c r="AD15" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE15" s="20" t="s">
         <v>92</v>
-      </c>
-      <c r="AE15" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="AF15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AG15" s="20" t="s">
+      <c r="AG15" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH15" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="AH15" s="20"/>
       <c r="AI15" s="20"/>
       <c r="AJ15" s="20"/>
       <c r="AK15" s="20"/>
       <c r="AL15" s="20"/>
       <c r="AM15" s="20"/>
       <c r="AN15" s="20"/>
-      <c r="AO15" s="10"/>
+      <c r="AO15" s="20"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
-    </row>
-    <row r="16" spans="2:52" ht="15" customHeight="1">
+      <c r="AS15" s="10"/>
+    </row>
+    <row r="16" spans="2:53" ht="15" customHeight="1">
       <c r="D16" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" t="s">
-        <v>219</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="H16" s="14"/>
+      <c r="I16" t="s">
+        <v>218</v>
+      </c>
+      <c r="M16" t="s">
         <v>100</v>
       </c>
-      <c r="Q16" s="15" t="s">
-        <v>60</v>
-      </c>
       <c r="R16" s="15" t="s">
         <v>60</v>
       </c>
       <c r="S16" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="15"/>
-      <c r="U16" s="16" t="s">
-        <v>61</v>
-      </c>
+      <c r="T16" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U16" s="15"/>
       <c r="V16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="W16" s="16"/>
-      <c r="AD16" s="22" t="s">
+      <c r="W16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="X16" s="16"/>
+      <c r="AE16" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="AG16" s="22" t="s">
+      <c r="AH16" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="AJ16" s="22" t="s">
+      <c r="AK16" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="AM16" s="22" t="s">
+      <c r="AN16" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="2:53" ht="15" customHeight="1">
+    <row r="17" spans="2:54" ht="15" customHeight="1">
       <c r="B17" s="10" t="s">
         <v>50</v>
       </c>
@@ -2216,57 +2255,55 @@
       <c r="E17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="H17" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="H17" t="s">
-        <v>219</v>
-      </c>
-      <c r="I17" s="10"/>
+      <c r="I17" t="s">
+        <v>218</v>
+      </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="10"/>
+      <c r="M17" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="M17" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="O17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="O17" s="15" t="s">
+      <c r="P17" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="Q17" s="10"/>
       <c r="R17" s="15" t="s">
         <v>60</v>
       </c>
       <c r="S17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="T17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U17" s="15"/>
       <c r="V17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="W17" s="15"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="15" t="s">
+      <c r="W17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB17" s="15" t="s">
-        <v>60</v>
+      <c r="AA17" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="AC17" s="15" t="s">
         <v>60</v>
@@ -2283,301 +2320,315 @@
       <c r="AG17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AH17" s="15"/>
+      <c r="AH17" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AI17" s="15"/>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>
       <c r="AL17" s="15"/>
       <c r="AM17" s="15"/>
       <c r="AN17" s="15"/>
-      <c r="AO17" s="10"/>
-      <c r="AP17" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="10"/>
       <c r="AQ17" s="15" t="s">
         <v>60</v>
       </c>
       <c r="AR17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AS17" s="10"/>
+      <c r="AS17" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AT17" s="10"/>
       <c r="AU17" s="10"/>
       <c r="AV17" s="10"/>
-      <c r="AX17" s="10"/>
-      <c r="AY17" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AW17" s="10"/>
+      <c r="AY17" s="10"/>
       <c r="AZ17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="BA17" s="10"/>
-    </row>
-    <row r="18" spans="2:53" ht="15" customHeight="1">
+      <c r="BA17" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="BB17" s="10"/>
+    </row>
+    <row r="18" spans="2:54" ht="15" customHeight="1">
       <c r="D18" s="10" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" t="s">
-        <v>219</v>
-      </c>
-      <c r="L18" s="10" t="s">
+      <c r="H18" s="14"/>
+      <c r="I18" t="s">
+        <v>218</v>
+      </c>
+      <c r="M18" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:53" ht="15" customHeight="1">
+    <row r="19" spans="2:54" ht="15" customHeight="1">
       <c r="D19" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="H19" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="H19" t="s">
-        <v>219</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="I19" t="s">
+        <v>218</v>
+      </c>
+      <c r="M19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="2:53" ht="15" customHeight="1">
-      <c r="D20" s="12" t="s">
+    <row r="20" spans="2:54" ht="15" customHeight="1">
+      <c r="D20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="H20" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H20" t="s">
-        <v>219</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="I20" t="s">
+        <v>218</v>
+      </c>
+      <c r="M20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="2:53" ht="15" customHeight="1">
-      <c r="D21" s="12" t="s">
+    <row r="21" spans="2:54" ht="15" customHeight="1">
+      <c r="D21" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" t="s">
-        <v>219</v>
-      </c>
-      <c r="L21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="2:53" ht="15" customHeight="1">
+      <c r="I21" t="s">
+        <v>218</v>
+      </c>
+      <c r="M21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="2:54" ht="15" customHeight="1">
       <c r="D22" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="H22" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="I22" t="s">
+        <v>218</v>
+      </c>
+      <c r="M22" t="s">
         <v>118</v>
       </c>
-      <c r="H22" t="s">
-        <v>219</v>
-      </c>
-      <c r="L22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="2:54" ht="15" customHeight="1">
       <c r="D23" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="I23" t="s">
+        <v>218</v>
+      </c>
+      <c r="M23" t="s">
         <v>121</v>
       </c>
-      <c r="H23" t="s">
-        <v>219</v>
-      </c>
-      <c r="L23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="2:54" ht="15" customHeight="1">
       <c r="D24" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="H24" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="I24" t="s">
+        <v>218</v>
+      </c>
+      <c r="M24" t="s">
         <v>125</v>
       </c>
-      <c r="H24" t="s">
-        <v>219</v>
-      </c>
-      <c r="L24" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="2:54" ht="15" customHeight="1">
       <c r="D25" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E25" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="H25" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="I25" t="s">
+        <v>218</v>
+      </c>
+      <c r="M25" t="s">
         <v>129</v>
       </c>
-      <c r="H25" t="s">
-        <v>219</v>
-      </c>
-      <c r="L25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="26" spans="2:54" ht="15" customHeight="1">
       <c r="D26" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F26" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H26" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="I26" t="s">
+        <v>218</v>
+      </c>
+      <c r="M26" t="s">
         <v>132</v>
       </c>
-      <c r="H26" t="s">
-        <v>219</v>
-      </c>
-      <c r="L26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="27" spans="2:54" ht="15" customHeight="1">
       <c r="D27" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="H27" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="I27" t="s">
+        <v>218</v>
+      </c>
+      <c r="M27" t="s">
         <v>136</v>
       </c>
-      <c r="H27" t="s">
-        <v>219</v>
-      </c>
-      <c r="L27" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="28" spans="2:54" ht="15" customHeight="1">
       <c r="D28" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F28" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="I28" t="s">
+        <v>218</v>
+      </c>
+      <c r="M28" t="s">
         <v>139</v>
       </c>
-      <c r="H28" t="s">
-        <v>219</v>
-      </c>
-      <c r="L28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="29" spans="2:54" ht="15" customHeight="1">
       <c r="D29" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="H29" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="I29" t="s">
+        <v>218</v>
+      </c>
+      <c r="M29" t="s">
         <v>143</v>
       </c>
-      <c r="H29" t="s">
-        <v>219</v>
-      </c>
-      <c r="L29" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q29" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="R29" s="10" t="s">
         <v>61</v>
       </c>
       <c r="S29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="V29" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="W29" s="15"/>
-      <c r="X29" s="10"/>
-      <c r="Y29" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="T29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W29" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="10"/>
       <c r="Z29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AA29" s="10"/>
-      <c r="AB29" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AA29" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB29" s="10"/>
       <c r="AC29" s="10" t="s">
         <v>61</v>
       </c>
@@ -2593,23 +2644,23 @@
       <c r="AG29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AH29" s="10"/>
+      <c r="AH29" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="AI29" s="10"/>
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="10"/>
       <c r="AM29" s="10"/>
       <c r="AN29" s="10"/>
-      <c r="AP29" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AO29" s="10"/>
       <c r="AQ29" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AR29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AT29" s="10" t="s">
+      <c r="AS29" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AU29" s="10" t="s">
@@ -2621,67 +2672,68 @@
       <c r="AW29" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="2:53" ht="15" customHeight="1">
+      <c r="AX29" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="2:54" ht="15" customHeight="1">
       <c r="D30" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E30" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="H30" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="I30" t="s">
+        <v>218</v>
+      </c>
+      <c r="J30" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H30" t="s">
-        <v>219</v>
-      </c>
-      <c r="I30" s="10" t="s">
+      <c r="K30" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="L30" s="10"/>
+      <c r="M30" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="N30" s="10"/>
+      <c r="N30" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
-      <c r="Q30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="Q30" s="10"/>
       <c r="R30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="S30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="V30" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="W30" s="15"/>
-      <c r="X30" s="10"/>
-      <c r="Y30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="T30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W30" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="10"/>
       <c r="Z30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AA30" s="10"/>
-      <c r="AB30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AA30" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB30" s="10"/>
       <c r="AC30" s="10" t="s">
         <v>61</v>
       </c>
@@ -2697,7 +2749,9 @@
       <c r="AG30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AH30" s="10"/>
+      <c r="AH30" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="AI30" s="10"/>
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
@@ -2705,16 +2759,14 @@
       <c r="AM30" s="10"/>
       <c r="AN30" s="10"/>
       <c r="AO30" s="10"/>
-      <c r="AP30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="AP30" s="10"/>
       <c r="AQ30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AR30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AT30" s="10" t="s">
+      <c r="AS30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="AU30" s="10" t="s">
@@ -2726,102 +2778,106 @@
       <c r="AW30" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="2:53" ht="15" customHeight="1">
+      <c r="AX30" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="2:54" ht="15" customHeight="1">
       <c r="D31" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="H31" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="I31" t="s">
+        <v>218</v>
+      </c>
+      <c r="M31" t="s">
         <v>153</v>
       </c>
-      <c r="H31" t="s">
-        <v>219</v>
-      </c>
-      <c r="L31" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="32" spans="2:53" ht="15" customHeight="1">
+    </row>
+    <row r="32" spans="2:54" ht="15" customHeight="1">
       <c r="D32" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F32" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="H32" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="I32" t="s">
+        <v>218</v>
+      </c>
+      <c r="M32" t="s">
         <v>156</v>
       </c>
-      <c r="H32" t="s">
-        <v>219</v>
-      </c>
-      <c r="L32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="2:52" ht="15" customHeight="1">
+    </row>
+    <row r="33" spans="2:53" ht="15" customHeight="1">
       <c r="D33" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E33" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="H33" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="I33" t="s">
+        <v>218</v>
+      </c>
+      <c r="M33" t="s">
         <v>160</v>
       </c>
-      <c r="H33" t="s">
-        <v>219</v>
-      </c>
-      <c r="L33" t="s">
+    </row>
+    <row r="34" spans="2:53" ht="15" customHeight="1">
+      <c r="B34" t="s">
+        <v>224</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="2:52" ht="15" customHeight="1">
-      <c r="B34" t="s">
-        <v>225</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="10"/>
+      <c r="G34" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="G34" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="H34" t="s">
-        <v>219</v>
-      </c>
       <c r="I34" t="s">
-        <v>227</v>
-      </c>
-      <c r="L34" t="s">
-        <v>223</v>
+        <v>218</v>
+      </c>
+      <c r="J34" t="s">
+        <v>226</v>
       </c>
       <c r="M34" t="s">
         <v>222</v>
       </c>
       <c r="N34" t="s">
-        <v>60</v>
+        <v>221</v>
       </c>
       <c r="O34" t="s">
         <v>60</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="P34" t="s">
         <v>60</v>
       </c>
       <c r="R34" t="s">
@@ -2834,23 +2890,23 @@
         <v>60</v>
       </c>
       <c r="U34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V34" t="s">
         <v>61</v>
       </c>
       <c r="W34" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y34" t="s">
+        <v>61</v>
+      </c>
+      <c r="X34" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z34" t="s">
         <v>62</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="AA34" t="s">
         <v>63</v>
       </c>
-      <c r="AB34" t="s">
-        <v>60</v>
-      </c>
       <c r="AC34" t="s">
         <v>60</v>
       </c>
@@ -2867,7 +2923,7 @@
         <v>60</v>
       </c>
       <c r="AH34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AI34" t="s">
         <v>61</v>
@@ -2884,14 +2940,17 @@
       <c r="AM34" t="s">
         <v>61</v>
       </c>
-      <c r="AY34" t="s">
-        <v>60</v>
+      <c r="AN34" t="s">
+        <v>61</v>
       </c>
       <c r="AZ34" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="35" spans="2:52" ht="15" customHeight="1">
+        <v>60</v>
+      </c>
+      <c r="BA34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="2:53" ht="15" customHeight="1">
       <c r="B35" s="10" t="s">
         <v>84</v>
       </c>
@@ -2899,382 +2958,395 @@
         <v>43269</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E35" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="H35" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="G35" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="H35" t="s">
-        <v>219</v>
-      </c>
-      <c r="I35" s="10"/>
+      <c r="I35" t="s">
+        <v>218</v>
+      </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
-      <c r="L35" s="15" t="s">
+      <c r="L35" s="10"/>
+      <c r="M35" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15" t="s">
+      <c r="P35" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="O35" s="15" t="s">
+      <c r="Q35" s="10"/>
+      <c r="R35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="S35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="T35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W35" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA35" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD35" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="R35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="S35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="V35" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="W35" s="15"/>
-      <c r="X35" s="10"/>
-      <c r="Y35" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z35" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA35" s="10"/>
-      <c r="AB35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC35" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD35" s="15" t="s">
-        <v>60</v>
-      </c>
       <c r="AE35" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="AF35" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="AG35" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH35" s="15"/>
+      <c r="AF35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG35" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH35" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AI35" s="15"/>
       <c r="AJ35" s="15"/>
       <c r="AK35" s="15"/>
       <c r="AL35" s="15"/>
       <c r="AM35" s="15"/>
       <c r="AN35" s="15"/>
-      <c r="AO35" s="10"/>
+      <c r="AO35" s="15"/>
       <c r="AP35" s="10"/>
       <c r="AQ35" s="10"/>
       <c r="AR35" s="10"/>
-      <c r="AZ35" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="36" spans="2:52" ht="15" customHeight="1">
+      <c r="AS35" s="10"/>
+      <c r="BA35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="2:53" ht="15" customHeight="1">
       <c r="D36" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="H36" t="s">
-        <v>219</v>
-      </c>
-      <c r="L36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="2:52" ht="15" customHeight="1">
+      <c r="I36" t="s">
+        <v>218</v>
+      </c>
+      <c r="M36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="2:53" ht="15" customHeight="1">
       <c r="D37" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="F37" s="10"/>
       <c r="G37" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="H37" t="s">
-        <v>219</v>
-      </c>
-      <c r="L37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="2:52" ht="15" customHeight="1">
+      <c r="H37" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" t="s">
+        <v>218</v>
+      </c>
+      <c r="M37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="2:53" ht="15" customHeight="1">
       <c r="D38" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="10"/>
+      <c r="G38" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H38" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="I38" t="s">
+        <v>218</v>
+      </c>
+      <c r="M38" t="s">
         <v>177</v>
       </c>
-      <c r="H38" t="s">
-        <v>219</v>
-      </c>
-      <c r="L38" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="39" spans="2:52" ht="15" customHeight="1">
+    </row>
+    <row r="39" spans="2:53" ht="15" customHeight="1">
       <c r="D39" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H39" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="H39" t="s">
-        <v>219</v>
-      </c>
-      <c r="L39" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="40" spans="2:52" ht="15" customHeight="1">
+      <c r="I39" t="s">
+        <v>218</v>
+      </c>
+      <c r="M39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="2:53" ht="15" customHeight="1">
       <c r="D40" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="10"/>
+      <c r="G40" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="H40" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="G40" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="H40" t="s">
-        <v>219</v>
-      </c>
-      <c r="L40" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="2:52" ht="15" customHeight="1">
+      <c r="I40" t="s">
+        <v>218</v>
+      </c>
+      <c r="M40" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="2:53" ht="15" customHeight="1">
       <c r="D41" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="10"/>
+      <c r="G41" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="H41" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="I41" t="s">
+        <v>218</v>
+      </c>
+      <c r="M41" t="s">
         <v>184</v>
       </c>
-      <c r="H41" t="s">
-        <v>219</v>
-      </c>
-      <c r="L41" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="2:52" ht="15" customHeight="1">
+    </row>
+    <row r="42" spans="2:53" ht="15" customHeight="1">
       <c r="D42" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="10"/>
+      <c r="G42" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="I42" t="s">
+        <v>218</v>
+      </c>
+      <c r="M42" t="s">
         <v>187</v>
       </c>
-      <c r="H42" t="s">
-        <v>219</v>
-      </c>
-      <c r="L42" t="s">
+    </row>
+    <row r="43" spans="2:53" ht="15" customHeight="1">
+      <c r="D43" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="43" spans="2:52" ht="15" customHeight="1">
-      <c r="D43" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E43" s="10" t="s">
+      <c r="F43" s="10"/>
+      <c r="G43" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="H43" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="I43" t="s">
+        <v>218</v>
+      </c>
+      <c r="M43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="2:53" ht="15" customHeight="1">
+      <c r="D44" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="H43" t="s">
-        <v>219</v>
-      </c>
-      <c r="L43" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="2:52" ht="15" customHeight="1">
-      <c r="D44" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="H44" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="I44" t="s">
+        <v>218</v>
+      </c>
+      <c r="M44" t="s">
         <v>194</v>
       </c>
-      <c r="H44" t="s">
-        <v>219</v>
-      </c>
-      <c r="L44" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="2:52" ht="15" customHeight="1">
+    </row>
+    <row r="45" spans="2:53" ht="15" customHeight="1">
       <c r="D45" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E45" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="H45" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="I45" t="s">
+        <v>218</v>
+      </c>
+      <c r="M45" t="s">
         <v>198</v>
       </c>
-      <c r="H45" t="s">
-        <v>219</v>
-      </c>
-      <c r="L45" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="2:52" ht="15" customHeight="1">
+    </row>
+    <row r="46" spans="2:53" ht="15" customHeight="1">
       <c r="B46" s="10"/>
       <c r="C46" s="11">
         <v>43273</v>
       </c>
       <c r="D46" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="F46" s="10"/>
+      <c r="G46" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="H46" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="G46" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="H46" t="s">
-        <v>219</v>
-      </c>
-      <c r="I46" s="10"/>
+      <c r="I46" t="s">
+        <v>218</v>
+      </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
-      <c r="L46" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="M46" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="N46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="N46" s="15" t="s">
+        <v>203</v>
+      </c>
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
-      <c r="Q46" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="Q46" s="10"/>
       <c r="R46" s="15" t="s">
         <v>60</v>
       </c>
       <c r="S46" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T46" s="15"/>
-      <c r="U46" s="15" t="s">
-        <v>61</v>
-      </c>
+      <c r="T46" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U46" s="15"/>
       <c r="V46" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="W46" s="15"/>
-      <c r="X46" s="10"/>
-      <c r="Y46" s="15" t="s">
+      <c r="W46" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="Z46" s="15" t="s">
+      <c r="AA46" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AA46" s="10"/>
-      <c r="AB46" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC46" s="10"/>
-      <c r="AD46" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO46" s="10"/>
+      <c r="AB46" s="10"/>
+      <c r="AC46" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD46" s="10"/>
+      <c r="AE46" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="AP46" s="10"/>
       <c r="AQ46" s="10"/>
       <c r="AR46" s="10"/>
-    </row>
-    <row r="47" spans="2:52" ht="15" customHeight="1">
+      <c r="AS46" s="10"/>
+    </row>
+    <row r="47" spans="2:53" ht="15" customHeight="1">
       <c r="D47" s="10" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="G47" s="14" t="s">
+      <c r="I47" t="s">
+        <v>218</v>
+      </c>
+      <c r="M47" t="s">
         <v>206</v>
       </c>
-      <c r="H47" t="s">
-        <v>219</v>
-      </c>
-      <c r="L47" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="48" spans="2:52" ht="15" customHeight="1">
+    </row>
+    <row r="48" spans="2:53" ht="15" customHeight="1">
       <c r="B48" s="10" t="s">
         <v>84</v>
       </c>
@@ -3282,159 +3354,163 @@
         <v>43278</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="10"/>
+      <c r="G48" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H48" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="I48" t="s">
+        <v>218</v>
+      </c>
+      <c r="M48" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="H48" t="s">
-        <v>219</v>
-      </c>
-      <c r="L48" s="15" t="s">
+      <c r="N48" s="15"/>
+      <c r="O48" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15" t="s">
+      <c r="P48" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="O48" s="15" t="s">
+      <c r="Q48" s="10"/>
+      <c r="R48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="S48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="T48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W48" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="10"/>
+      <c r="Z48" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA48" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB48" s="10"/>
+      <c r="AC48" s="10"/>
+      <c r="AD48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE48" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF48" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="R48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="S48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V48" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="W48" s="15"/>
-      <c r="X48" s="10"/>
-      <c r="Y48" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z48" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA48" s="10"/>
-      <c r="AB48" s="10"/>
-      <c r="AC48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD48" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE48" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="AG48" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="AH48" s="15"/>
+      <c r="AH48" s="23" t="s">
+        <v>213</v>
+      </c>
       <c r="AI48" s="15"/>
       <c r="AJ48" s="15"/>
       <c r="AK48" s="15"/>
       <c r="AL48" s="15"/>
       <c r="AM48" s="15"/>
       <c r="AN48" s="15"/>
-      <c r="AO48" s="10"/>
-      <c r="AP48" s="15" t="s">
-        <v>60</v>
-      </c>
+      <c r="AO48" s="15"/>
+      <c r="AP48" s="10"/>
       <c r="AQ48" s="15" t="s">
         <v>60</v>
       </c>
       <c r="AR48" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="2:52" ht="15" customHeight="1">
+      <c r="AS48" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="2:53" ht="15" customHeight="1">
       <c r="D49" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="10"/>
+      <c r="G49" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="I49" t="s">
+        <v>218</v>
+      </c>
+      <c r="M49" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="2:53" ht="15" customHeight="1">
+      <c r="D50" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="G49" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="H49" t="s">
-        <v>219</v>
-      </c>
-      <c r="L49" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="50" spans="2:52" ht="15" customHeight="1">
-      <c r="D50" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="H50" t="s">
-        <v>219</v>
-      </c>
-      <c r="I50" s="10"/>
+      <c r="H50" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="I50" t="s">
+        <v>218</v>
+      </c>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
-      <c r="L50" t="s">
-        <v>216</v>
-      </c>
-      <c r="AY50" s="15" t="s">
-        <v>60</v>
+      <c r="L50" s="10"/>
+      <c r="M50" t="s">
+        <v>215</v>
       </c>
       <c r="AZ50" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="51" spans="2:52" ht="15" customHeight="1">
+      <c r="BA50" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:53" ht="15" customHeight="1">
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>217</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="F51" s="10"/>
       <c r="G51" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="H51" t="s">
-        <v>219</v>
-      </c>
-      <c r="L51" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="52" spans="2:52" ht="15" customHeight="1">
+        <v>216</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="I51" t="s">
+        <v>218</v>
+      </c>
+      <c r="M51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="2:53" ht="15" customHeight="1">
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
       <c r="D52" s="24"/>
@@ -3450,9 +3526,9 @@
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:AZ51"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Alignement of LLC020 and GLEDOPTO to new template model.
</commit_message>
<xml_diff>
--- a/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
+++ b/resources/AbeilleDeamon/documentsDeDev/AbeilleEquipmentFunctionSupported.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="8660" windowWidth="64880" windowHeight="27260" tabRatio="500"/>
+    <workbookView xWindow="9880" yWindow="3520" windowWidth="64880" windowHeight="27260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="239">
   <si>
     <t>Inclusion</t>
   </si>
@@ -721,6 +721,24 @@
   </si>
   <si>
     <t>sensor_86sw2Un</t>
+  </si>
+  <si>
+    <t>GLEDOPTO</t>
+  </si>
+  <si>
+    <t>GLEDOPTO GU10 Dimmable 5W</t>
+  </si>
+  <si>
+    <t>3.0.e</t>
+  </si>
+  <si>
+    <t>En cours</t>
+  </si>
+  <si>
+    <t>Yes sur allumage la premiere fois ou apres reset</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
   </si>
 </sst>
 </file>
@@ -900,12 +918,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -981,7 +1011,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="25">
     <cellStyle name="40 % - Accent1" xfId="4" builtinId="31" customBuiltin="1"/>
     <cellStyle name="Bon" xfId="1" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27" customBuiltin="1"/>
@@ -989,10 +1019,22 @@
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Neutre" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
@@ -1326,7 +1368,7 @@
   <dimension ref="B2:BB52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="X53" sqref="X53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -2037,7 +2079,9 @@
       <c r="W13" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="X13" s="15"/>
+      <c r="X13" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="15" t="s">
         <v>62</v>
@@ -3511,22 +3555,69 @@
       </c>
     </row>
     <row r="52" spans="2:53" ht="15" customHeight="1">
-      <c r="B52" s="10"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="10"/>
+      <c r="B52" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C52" s="11">
+        <v>43432</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>236</v>
+      </c>
       <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
+      <c r="K52" s="10" t="s">
+        <v>237</v>
+      </c>
       <c r="L52" s="10"/>
-      <c r="M52" s="10"/>
+      <c r="M52" s="10" t="s">
+        <v>233</v>
+      </c>
       <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
+      <c r="O52" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="P52" s="10" t="s">
+        <v>238</v>
+      </c>
       <c r="Q52" s="10"/>
+      <c r="R52" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="S52" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="T52" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="U52" s="15"/>
+      <c r="V52" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="W52" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="X52" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z52" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA52" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>